<commit_message>
Next Day Update 2
Images loaded automatically, making add_imgs.js obsolete (except for initial population of page).
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\GitHub\jakobwonisch.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604EAFE9-22DC-4995-B83D-BA7A8FDB136A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866397C0-8939-40FD-8FD4-F62F51CC7B0D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -31,163 +31,166 @@
     <t>educational Workshops/Training/Mentoring</t>
   </si>
   <si>
+    <t>Costs (participants)</t>
+  </si>
+  <si>
+    <t>Online Courses (1= nur online)</t>
+  </si>
+  <si>
+    <t>Award</t>
+  </si>
+  <si>
+    <t>Eu</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Central America</t>
+  </si>
+  <si>
+    <t>Middle East</t>
+  </si>
+  <si>
+    <t>Agora</t>
+  </si>
+  <si>
+    <t>Belize, Costa Rica, El Salvador, Guatemala, Honduras, Dominican Rep., Mexico, Nicaragua, Panama, Cuba, Haiti, Peru, Chile, Argentinia, Brazil, Bolivia, Colombia, Ecuador, French Guinea, Paraguay, Uruguay, Venezuela, Puerto Rico</t>
+  </si>
+  <si>
+    <t>Alfanar</t>
+  </si>
+  <si>
+    <t>Egypt, Lebanon, Libya</t>
+  </si>
+  <si>
+    <t>AMANI Institute</t>
+  </si>
+  <si>
+    <t>India, Kenya, Brazil</t>
+  </si>
+  <si>
+    <t>Ashoka</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>Bonventure</t>
+  </si>
+  <si>
+    <t>Austria, Germany, Switzerland</t>
+  </si>
+  <si>
+    <t>Boost Aid for Social Entrepreneurship by Training (BASET)</t>
+  </si>
+  <si>
+    <t>Belgium, Bulgaria, Greece, UK</t>
+  </si>
+  <si>
+    <t>Centre for Social Innovation</t>
+  </si>
+  <si>
+    <t>Austria, Germany</t>
+  </si>
+  <si>
+    <t>Deshpande Foundation</t>
+  </si>
+  <si>
+    <t>Canada, USA, India</t>
+  </si>
+  <si>
+    <t>Echoing Green</t>
+  </si>
+  <si>
+    <t>Enactus</t>
+  </si>
+  <si>
+    <t>Australia, Azerbaijan, Brazil, Canada, China, France, Germany, Ghana, Guatemala, India, Ireland, Italy, Kazakhstan, Kenya, Korea, Kyrgyzstan,Malaysia, Mexico, Morocco, Netherlands, Nigeria, Philippines, Poland, Puerto Rico, Russia, Senegal, Singapore, South Africa, Swaziland, Tajikistan, Tunisia, Ukraine, United Kingdom, United States, Zimbabwe</t>
+  </si>
+  <si>
+    <t>Endeva</t>
+  </si>
+  <si>
+    <t>Algeria, Angola, Benin, Botswana, Burkina Faso, Burundi, Cabo Verde, Cameroon, Central African Republic, Chad, Comoros, Dem. Rep. Congo, Congo, Cote d’Ivoire, Djibouti, Egypt, Equatorial Guinea, Eritrea, Swaziland, Ethiopia, Gabon, Gambia, Ghana, Guinea, Guinea-Bissau, Kenya, Lesotho, Liberia, Libya, Madagascar, Malawi, Mali, Mauritania, Mauritius, Morocco, Mozambique, Namibia, Niger, Nigeria, Rwanda, Sao Tome and Principe, Senegal, Seychelles, Sierra Leone, Somalia, South Africa, South Sudan, Sudan, Tanzania, Togo, Tunisia, Uganda, Zambia, Zimbabwe, Haiti, Cuba, Dominican Rep., Europe, Argentinia, Brazil, Bolivia, Chile, Colombia, Costa Rica, Cuba, Dominican Rep., Ecuador, El Salvador, French Guiana, Guatemala, Honduras, Martinique, Mexico, Nicaragua, Panama, Paraguay, Peru, Puerto Rico, Uruguay, Venezuela, Algeria, Bahrain, Egypt, Iran, Iraq, Israel</t>
+  </si>
+  <si>
+    <t>Entrepreneurship School (Social Entrepreneurship)</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>Enviu</t>
+  </si>
+  <si>
+    <t>The Netherlands, Nairobi, Kenya, India, USA</t>
+  </si>
+  <si>
+    <t>Euforia</t>
+  </si>
+  <si>
+    <t>Switzerland, Rwanda, Egypt, Greece, Turkey, Austria, Netherlands, P. of Liechtenstein, France, Germany, Portugal, Colombia, Peru, Bolivia</t>
+  </si>
+  <si>
+    <t>European Social Innovation Competition</t>
+  </si>
+  <si>
+    <t>Iceland, Norway, Albania, Bosnia and Herzegovina, Macedonia, Montenegro, Serbia, Turkey, Israel, Moldova, Switzerland, Faroe Islands, Ukraine, Tunisia, Georgia, Armenia</t>
+  </si>
+  <si>
+    <t>EY - Entrepreneur of the Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, Indonesia, Phillipines </t>
+  </si>
+  <si>
+    <t>Facebook Social Entrepreneurship Award</t>
+  </si>
+  <si>
+    <t>Fledge</t>
+  </si>
+  <si>
+    <t>Peru, Spain, Italy, Canada, USA</t>
+  </si>
+  <si>
+    <t>Fossil Foundation</t>
+  </si>
+  <si>
+    <t>Canada, USA, Ecuador, Zambia, Kenya, Nigeria, Italy, Switzerland, UK, Poland, India, Cambodia, Laos, China, Hong Kong, Taiwan</t>
+  </si>
+  <si>
+    <t>Global Social Entrepreneurship Network</t>
+  </si>
+  <si>
+    <t>Canada, USA, Europe, Chile, South Africa, Tanzania, Congo, Chad, Morocco, Israel, Cyprus, China, Dem. Rep. Korea, Thailand, Malaysia, Indonesia, Australia, New Zealand, Taiwan</t>
+  </si>
+  <si>
     <t>Costs</t>
   </si>
   <si>
     <t>Online Courses (1= nur online, 2= beides)</t>
   </si>
   <si>
-    <t>Award</t>
-  </si>
-  <si>
-    <t>Eu</t>
-  </si>
-  <si>
-    <t>North America</t>
-  </si>
-  <si>
-    <t>South America</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Central America</t>
-  </si>
-  <si>
-    <t>Middle East</t>
-  </si>
-  <si>
-    <t>Agora</t>
-  </si>
-  <si>
-    <t>Belize, Costa Rica, El Salvador, Guatemala, Honduras, Dominican Rep., Mexico, Nicaragua, Panama, Cuba, Haiti, Peru, Chile, Argentinia, Brazil, Bolivia, Colombia, Ecuador, French Guinea, Paraguay, Uruguay, Venezuela, Puerto Rico</t>
-  </si>
-  <si>
-    <t>Alfanar</t>
-  </si>
-  <si>
-    <t>Egypt, Lebanon, Libya</t>
-  </si>
-  <si>
-    <t>Amani Institute</t>
-  </si>
-  <si>
-    <t>India, Kenya, Brazil</t>
-  </si>
-  <si>
-    <t>Ashoka</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>Bonventure</t>
-  </si>
-  <si>
-    <t>Austria, Germany, Switzerland</t>
-  </si>
-  <si>
-    <t>Boost Aid for Social Entrepreneurship by Training</t>
-  </si>
-  <si>
-    <t>Belgium, Bulgaria, Greece, UK</t>
-  </si>
-  <si>
-    <t>Centre for Social Innovation</t>
-  </si>
-  <si>
-    <t>Austria, Germany</t>
-  </si>
-  <si>
-    <t>Deshpande Foundation</t>
-  </si>
-  <si>
-    <t>Canada, USA, India</t>
-  </si>
-  <si>
-    <t>Echoing Green</t>
-  </si>
-  <si>
-    <t>Enactus</t>
-  </si>
-  <si>
-    <t>Australia, Azerbaijan, Brazil, Canada, China, France, Germany, Ghana, Guatemala, India, Ireland, Italy, Kazakhstan, Kenya, Korea, Kyrgyzstan,Malaysia, Mexico, Morocco, Netherlands, Nigeria, Philippines, Poland, Puerto Rico, Russia, Senegal, Singapore, South Africa, Swaziland, Tajikistan, Tunisia, Ukraine, United Kingdom, United States, Zimbabwe</t>
-  </si>
-  <si>
-    <t>Endeva</t>
-  </si>
-  <si>
-    <t>Africa, , Haiti, Cuba, Dominican Rep., Eastern Europe and the CIS, Europe, Latin America, MENA</t>
-  </si>
-  <si>
-    <t>Entrepreneurship School</t>
-  </si>
-  <si>
-    <t>online</t>
-  </si>
-  <si>
-    <t>Enviu</t>
-  </si>
-  <si>
-    <t>The Netherlands, Nairobi, Kenya, India, USA</t>
-  </si>
-  <si>
-    <t>Euforia</t>
-  </si>
-  <si>
-    <t>Switzerland, Rwanda, Egypt, Greece, Turkey, Austria, Netherlands, P. of Liechtenstein, France, Germany, Portugal, Colombia, Peru, Bolivia</t>
-  </si>
-  <si>
-    <t>European Social Innovation Competition</t>
-  </si>
-  <si>
-    <t>Iceland, Norway, Albania, Bosnia and Herzegovina, Macedonia, Montenegro, Serbia, Turkey, Israel, Moldova, Switzerland, Faroe Islands, Ukraine, Tunisia, Georgia, Armenia</t>
-  </si>
-  <si>
-    <t>EY - Entrepreneur of the Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, Indonesia, Phillipines </t>
-  </si>
-  <si>
-    <t>Facebook Social Entrepreneurship Award</t>
-  </si>
-  <si>
-    <t>Fledge</t>
-  </si>
-  <si>
-    <t>Peru, Spain, Italy, Canada, USA</t>
-  </si>
-  <si>
-    <t>Fossil Foundation</t>
-  </si>
-  <si>
-    <t>Canada, USA, Ecuador, Zambia, Kenya, Nigeria, Italy, Switzerland, UK, Poland, India, Cambodia, Laos, China, Hong Kong, Taiwan</t>
-  </si>
-  <si>
-    <t>Global Social Entrepreneurship Network</t>
-  </si>
-  <si>
-    <t>Canada, USA, Europe, Chile, South Africa, Tanzania, Congo, Chad, Morocco, Israel, Cyprus, China, Dem. Rep. Korea, Thailand, Malaysia, Indonesia, Australia, New Zealand, Taiwan</t>
-  </si>
-  <si>
     <t>Europe</t>
   </si>
   <si>
     <t>Global Social Venture Competition</t>
   </si>
   <si>
-    <t>65 countries (Mappe auf Website)</t>
-  </si>
-  <si>
-    <t>Global Center for Social Entrepreneurship Networks</t>
+    <t>Global Center for Social Entrepreneurship Networks (GCSEN)</t>
   </si>
   <si>
     <t xml:space="preserve">Halcyon </t>
@@ -214,37 +217,25 @@
     <t>USA, Canada, Mexico, Dominican Rep., Nicaragua, Guatemala, Trinidad and Tobago, Colombia, Argentinia, Paraguay, Brasil, Europe, Morocco, Tunisia, South Africa, Australia, Lebanon, Mali, Burkina Faso, Cote d'Ivoire, Senegal, Togo, Uganda, Kenya, Egypt, Turkey, Armenia, Teheran, Nepal, India, China, Myanmar, Cambodia, Vietnam, Malaysia, Singapore, Indonesia, Philippines, Dem. Rep. Korea, Japan, New Zealand</t>
   </si>
   <si>
-    <t>Masschallenge</t>
-  </si>
-  <si>
-    <t>1 (99 Dollars)</t>
+    <t>MassChallenge</t>
   </si>
   <si>
     <t>USA, Israel, Mexico, Switzerland, UK</t>
   </si>
   <si>
-    <t>Middlesex University Online Course</t>
-  </si>
-  <si>
-    <t>Miller Center for Social Entrepreneurship</t>
+    <t>Middlesex University London (Social Enterprise: Turning Ideas into Action)</t>
   </si>
   <si>
     <t>Ogunte</t>
   </si>
   <si>
-    <t>0 (individual coaching for a fee)</t>
-  </si>
-  <si>
     <t>Orange Social Venture Prize</t>
   </si>
   <si>
     <t>Morocco, Tunisia, Egypt, Senegal, Botswana, Liberia, Ivory Coast, Cameroon, Mali, Guinea Conakry, Guinea Bissau, Madagascar, Niger, Central African Republic, Democratic Republic of Congo, Jordan and Burkina Faso</t>
   </si>
   <si>
-    <t>PlusAcumen</t>
-  </si>
-  <si>
-    <t>1 (free and low cost)</t>
+    <t>Acumen</t>
   </si>
   <si>
     <t>Schwab Foundation for Social Entrepreneurship</t>
@@ -262,11 +253,10 @@
     <t xml:space="preserve">Colombia, India, Tanzania, Thailand, Uganda </t>
   </si>
   <si>
-    <t>Seed Stars</t>
-  </si>
-  <si>
-    <t>Afghanistan, Armenia, Azerbaijan, Bahrain, Bangladesh, Bhutan, Brunei, Cambodia, China, Cyprus, Georgia, India, Indonesia, Iran, Iraq, Israel, Japan, Jordan, Kazakhstan, Kuwait, Kyrgyzstan, Laos, Lebanon, Malaysia, Maldives, Mongolia, Myanmar, Nepal, North Korea, Oman, Pakistan, Palestine, Philippines, Qatar, Russia, Saudi Arabia, Singapore, South Korea, Sri Lanka, Syria, Taiwan, Tajikistan, Thailand, Timor-Leste, Turkey, Turkmenistan, United Arab Emirates, Uzbekistan, Vietnam, Yemen, 
-Yemen Africa, MENA, Latin America, ECA</t>
+    <t>Seedstars</t>
+  </si>
+  <si>
+    <t>Afghanistan, Armenia, Azerbaijan, Bahrain, Bangladesh, Bhutan, Brunei, Cambodia, China, Cyprus, Georgia, India, Indonesia, Iran, Iraq, Israel, Japan, Jordan, Kazakhstan, Kuwait, Kyrgyzstan, Laos, Lebanon, Malaysia, Maldives, Mongolia, Myanmar, Nepal, North Korea, Oman, Pakistan, Palestine, Philippines, Qatar, Russia, Saudi Arabia, Singapore, South Korea, Sri Lanka, Syria, Taiwan, Tajikistan, Thailand, Timor-Leste, Turkey, Turkmenistan, United Arab Emirates, Uzbekistan, Vietnam, Yemen, Algeria, Angola, Benin, Botswana, Burkina Faso, Burundi, Cabo Verde, Cameroon, Central African Republic, Chad, Comoros, Dem. Rep. Congo, Congo, Cote d’Ivoire, Djibouti, Egypt, Equatorial Guinea, Eritrea, Swaziland, Ethiopia, Gabon, Gambia, Ghana, Guinea, Guinea-Bissau, Kenya, Lesotho, Liberia, Libya, Madagascar, Malawi, Mali, Mauritania, Mauritius, Morocco, Mozambique, Namibia, Niger, Nigeria, Rwanda, Sao Tome and Principe, Senegal, Seychelles, Sierra Leone, Somalia, South Africa, South Sudan, Sudan, Tanzania, Togo, Tunisia, Uganda, Zambia, Zimbabwe, Algeria, Bahrain, Egypt, Iran, Iraq, Israel, Argentinia, Brazil, Bolivia, Chile, Colombia, Costa Rica, Cuba, Dominican Rep., Ecuador, El Salvador, French Guiana, Guatemala, Honduras, Martinique, Mexico, Nicaragua, Panama, Paraguay, Peru, Puerto Rico, Uruguay, Venezuela, Albania, Armenia, Azerbaijan, Belarus, Georgia, Kazakhstan, Kosovo, Kyrgyzstan, Macedonia, Moldova, Montenegro, Russia, Serbia, Tajikistan, Turkmenistan, Ukraine, Uzbekistan</t>
   </si>
   <si>
     <t>Segal Family Foundation</t>
@@ -302,7 +292,7 @@
     <t>Guatemala, Ecuador, Dominican Rep., Nicaragua</t>
   </si>
   <si>
-    <t>Society Profits</t>
+    <t>SocietyProfits</t>
   </si>
   <si>
     <t>Taproot Foundation</t>
@@ -332,6 +322,9 @@
     <t>Uncharted</t>
   </si>
   <si>
+    <t>(no information)</t>
+  </si>
+  <si>
     <t>UnLtd</t>
   </si>
   <si>
@@ -374,7 +367,7 @@
     <t>Australia, Kenya, Nigeria, South Africa, Columbia, USA</t>
   </si>
   <si>
-    <t>global, online</t>
+    <t>Miller Center for Social Entrepreneurship - Global Social Benefit Institute</t>
   </si>
 </sst>
 </file>
@@ -402,18 +395,12 @@
       <name val="HelvNeue55"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF93C47D"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -448,7 +435,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,12 +753,12 @@
   <dimension ref="A1:O996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="38.796875" customWidth="1"/>
+    <col min="1" max="1" width="19.3984375" customWidth="1"/>
     <col min="2" max="2" width="8.296875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="11.69921875" customWidth="1"/>
@@ -932,7 +919,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4">
@@ -1073,7 +1060,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="4">
@@ -1355,7 +1342,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="4">
@@ -1788,16 +1775,16 @@
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>7</v>
@@ -1823,7 +1810,7 @@
     </row>
     <row r="23" spans="1:15" ht="19.5" customHeight="1">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -1865,12 +1852,12 @@
         <v>1</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="19.5" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="4">
         <v>0</v>
@@ -1917,7 +1904,7 @@
     </row>
     <row r="25" spans="1:15" ht="19.5" customHeight="1">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -1959,12 +1946,12 @@
         <v>1</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="19.5" customHeight="1">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -2011,7 +1998,7 @@
     </row>
     <row r="27" spans="1:15" ht="19.5" customHeight="1">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -2058,7 +2045,7 @@
     </row>
     <row r="28" spans="1:15" ht="19.5" customHeight="1">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -2100,12 +2087,12 @@
         <v>0</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="19.5" customHeight="1">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" s="4">
         <v>0</v>
@@ -2147,12 +2134,12 @@
         <v>1</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A30" t="s">
-        <v>64</v>
+      <c r="A30" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
@@ -2160,8 +2147,8 @@
       <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>65</v>
+      <c r="D30" s="4">
+        <v>1</v>
       </c>
       <c r="E30" s="4">
         <v>0</v>
@@ -2198,7 +2185,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="4">
@@ -2245,8 +2232,8 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A32" t="s">
-        <v>68</v>
+      <c r="A32" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
@@ -2293,7 +2280,7 @@
     </row>
     <row r="33" spans="1:15" ht="19.5" customHeight="1">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="4">
         <v>0</v>
@@ -2301,8 +2288,8 @@
       <c r="C33" s="4">
         <v>1</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>70</v>
+      <c r="D33" s="4">
+        <v>0</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
@@ -2335,60 +2322,60 @@
         <v>1</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="19.5" customHeight="1">
       <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4">
+        <v>1</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4">
+        <v>0</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4">
-        <v>0</v>
-      </c>
-      <c r="I34" s="4">
-        <v>0</v>
-      </c>
-      <c r="J34" s="4">
-        <v>1</v>
-      </c>
-      <c r="K34" s="4">
-        <v>0</v>
-      </c>
-      <c r="L34" s="4">
-        <v>0</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0</v>
-      </c>
-      <c r="N34" s="4">
-        <v>1</v>
-      </c>
-      <c r="O34" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
       <c r="B35" s="4">
         <v>0</v>
       </c>
@@ -2398,8 +2385,8 @@
       <c r="D35" s="4">
         <v>1</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>74</v>
+      <c r="E35" s="4">
+        <v>1</v>
       </c>
       <c r="F35" s="4">
         <v>0</v>
@@ -2434,7 +2421,7 @@
     </row>
     <row r="36" spans="1:15" ht="19.5" customHeight="1">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
@@ -2481,7 +2468,7 @@
     </row>
     <row r="37" spans="1:15" ht="19.5" customHeight="1">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
@@ -2523,106 +2510,106 @@
         <v>0</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="19.5" customHeight="1">
       <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>1</v>
+      </c>
+      <c r="J38" s="4">
+        <v>1</v>
+      </c>
+      <c r="K38" s="4">
+        <v>0</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1</v>
+      </c>
+      <c r="M38" s="4">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4">
+        <v>0</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4">
+        <v>1</v>
+      </c>
+      <c r="K39" s="4">
+        <v>0</v>
+      </c>
+      <c r="L39" s="4">
+        <v>1</v>
+      </c>
+      <c r="M39" s="4">
+        <v>1</v>
+      </c>
+      <c r="N39" s="4">
+        <v>1</v>
+      </c>
+      <c r="O39" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4">
-        <v>1</v>
-      </c>
-      <c r="F38" s="4">
-        <v>1</v>
-      </c>
-      <c r="G38" s="4">
-        <v>0</v>
-      </c>
-      <c r="H38" s="4">
-        <v>0</v>
-      </c>
-      <c r="I38" s="4">
-        <v>1</v>
-      </c>
-      <c r="J38" s="4">
-        <v>1</v>
-      </c>
-      <c r="K38" s="4">
-        <v>0</v>
-      </c>
-      <c r="L38" s="4">
-        <v>1</v>
-      </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4">
-        <v>1</v>
-      </c>
-      <c r="G39" s="4">
-        <v>1</v>
-      </c>
-      <c r="H39" s="4">
-        <v>0</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1</v>
-      </c>
-      <c r="J39" s="4">
-        <v>1</v>
-      </c>
-      <c r="K39" s="4">
-        <v>0</v>
-      </c>
-      <c r="L39" s="4">
-        <v>1</v>
-      </c>
-      <c r="M39" s="4">
-        <v>1</v>
-      </c>
-      <c r="N39" s="4">
-        <v>1</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="19.5" customHeight="1">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
@@ -2664,12 +2651,12 @@
         <v>0</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="19.5" customHeight="1">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -2716,7 +2703,7 @@
     </row>
     <row r="42" spans="1:15" ht="19.5" customHeight="1">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B42" s="4">
         <v>0</v>
@@ -2763,7 +2750,7 @@
     </row>
     <row r="43" spans="1:15" ht="19.5" customHeight="1">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B43" s="4">
         <v>0</v>
@@ -2805,12 +2792,54 @@
         <v>0</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="19.5" customHeight="1">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4">
+        <v>1</v>
+      </c>
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
+      <c r="K44" s="4">
+        <v>1</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+      <c r="M44" s="4">
+        <v>1</v>
+      </c>
+      <c r="N44" s="4">
+        <v>1</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="19.5" customHeight="1">
@@ -2824,16 +2853,16 @@
         <v>2</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>7</v>
@@ -2859,7 +2888,7 @@
     </row>
     <row r="46" spans="1:15" ht="19.5" customHeight="1">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B46" s="4">
         <v>0</v>
@@ -2901,12 +2930,12 @@
         <v>1</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="19.5" customHeight="1">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B47" s="4">
         <v>0</v>
@@ -2948,12 +2977,12 @@
         <v>0</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A48" t="s">
-        <v>93</v>
+      <c r="A48" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="B48" s="4">
         <v>0</v>
@@ -3000,7 +3029,7 @@
     </row>
     <row r="49" spans="1:15" ht="19.5" customHeight="1">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B49" s="4">
         <v>0</v>
@@ -3047,7 +3076,7 @@
     </row>
     <row r="50" spans="1:15" ht="19.5" customHeight="1">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -3089,12 +3118,12 @@
         <v>1</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="19.5" customHeight="1">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B51" s="4">
         <v>0</v>
@@ -3136,12 +3165,12 @@
         <v>0</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="19.5" customHeight="1">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B52" s="4">
         <v>0</v>
@@ -3183,12 +3212,12 @@
         <v>0</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="19.5" customHeight="1">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
@@ -3235,7 +3264,7 @@
     </row>
     <row r="54" spans="1:15" ht="19.5" customHeight="1">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -3251,11 +3280,14 @@
       </c>
       <c r="F54" s="4">
         <v>0</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="19.5" customHeight="1">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
@@ -3297,12 +3329,12 @@
         <v>0</v>
       </c>
       <c r="O55" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="19.5" customHeight="1">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
@@ -3349,7 +3381,7 @@
     </row>
     <row r="57" spans="1:15" ht="19.5" customHeight="1">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
@@ -3396,7 +3428,7 @@
     </row>
     <row r="58" spans="1:15" ht="19.5" customHeight="1">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
@@ -3438,12 +3470,12 @@
         <v>0</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="19.5" customHeight="1">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
@@ -3490,7 +3522,7 @@
     </row>
     <row r="60" spans="1:15" ht="19.5" customHeight="1">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B60" s="4">
         <v>0</v>
@@ -3532,12 +3564,12 @@
         <v>0</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="19.5" customHeight="1">
       <c r="A61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
@@ -3579,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="O61" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="15.75" customHeight="1">
@@ -3593,16 +3625,16 @@
         <v>2</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>7</v>
@@ -3614,7 +3646,7 @@
         <v>9</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>11</v>
@@ -3628,7 +3660,7 @@
     </row>
     <row r="63" spans="1:15" ht="15.75" customHeight="1">
       <c r="A63" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B63" s="4">
         <v>1</v>
@@ -3670,7 +3702,7 @@
         <v>0</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="15.75" customHeight="1"/>

</xml_diff>